<commit_message>
add questions texts to questions.xls
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -13,6 +13,198 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>xoposhiy</author>
+  </authors>
+  <commentList>
+    <comment ref="J4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Бесплатная медицина и бесплатное образование относятся к числу важнейших, неприкосновенных социальных гарантий</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Государства бывшего СССР относятся к сфере особых внешнеполитических интересов России.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>России нужны более высокие таможенные пошлины для защиты отечественного производителя в целом ряде отраслей экономики.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Необходим пересмотр итогов приватизации. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Государственные корпорации — это эффективный инструмент управления стратегическими отраслями национальной экономики.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>В Конституции Российской Федерации должен быть закреплен особый статус русских как титульной нации</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Трудовая миграция иностранных граждан должна быть строго ограничена.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Плоская ставка подоходного налога должна сохраняться в течение длительного времени</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Единый государственный экзамен (ЕГЭ), при должном качестве администрирования, является оптимальной формой конкурсного отбора студентов вузов.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Россия должна стремиться к тесной политической и экономической интеграции с Евросоюзом.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Существенная часть трудовой пенсии должна формироваться из накопительной части.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Роль государства в экономике должна быть сведена к минимуму. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Российская армия должна формироваться исключительно на контрактной основе.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52,7 +244,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +306,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -233,9 +432,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -252,9 +448,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,6 +486,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -596,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA172"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="A131" sqref="A131:XFD132"/>
     </sheetView>
   </sheetViews>
@@ -618,83 +817,83 @@
     <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="13" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="12">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12">
+    <row r="1" spans="1:26" s="12" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11">
         <v>3</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="11">
         <v>4</v>
       </c>
-      <c r="F1" s="12">
+      <c r="F1" s="11">
         <v>5</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="11">
         <v>6</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="11">
         <v>7</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="11">
         <v>8</v>
       </c>
-      <c r="J1" s="12">
+      <c r="J1" s="11">
         <v>9</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="11">
         <v>10</v>
       </c>
-      <c r="L1" s="12">
+      <c r="L1" s="11">
         <v>11</v>
       </c>
-      <c r="M1" s="12">
+      <c r="M1" s="11">
         <v>12</v>
       </c>
-      <c r="N1" s="12">
+      <c r="N1" s="11">
         <v>13</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="11">
         <v>14</v>
       </c>
-      <c r="P1" s="12">
+      <c r="P1" s="11">
         <v>15</v>
       </c>
-      <c r="Q1" s="12">
+      <c r="Q1" s="11">
         <v>16</v>
       </c>
-      <c r="R1" s="12">
+      <c r="R1" s="11">
         <v>17</v>
       </c>
-      <c r="S1" s="12">
+      <c r="S1" s="11">
         <v>18</v>
       </c>
-      <c r="T1" s="12">
+      <c r="T1" s="11">
         <v>19</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="11">
         <v>20</v>
       </c>
-      <c r="V1" s="12">
+      <c r="V1" s="11">
         <v>21</v>
       </c>
-      <c r="W1" s="12">
+      <c r="W1" s="11">
         <v>22</v>
       </c>
-      <c r="X1" s="12">
+      <c r="X1" s="11">
         <v>23</v>
       </c>
-      <c r="Y1" s="12">
+      <c r="Y1" s="11">
         <v>24</v>
       </c>
-      <c r="Z1" s="12">
+      <c r="Z1" s="11">
         <v>25</v>
       </c>
     </row>
@@ -9862,7 +10061,7 @@
       </c>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A122" s="14" t="s">
+      <c r="A122" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B122" s="5">
@@ -9967,7 +10166,7 @@
       </c>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A123" s="14" t="s">
+      <c r="A123" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B123" s="5">
@@ -10072,7 +10271,7 @@
       </c>
     </row>
     <row r="124" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A124" s="14" t="s">
+      <c r="A124" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B124" s="5">
@@ -10177,7 +10376,7 @@
       </c>
     </row>
     <row r="125" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A125" s="14" t="s">
+      <c r="A125" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B125" s="1">
@@ -10282,7 +10481,7 @@
       </c>
     </row>
     <row r="126" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A126" s="14" t="s">
+      <c r="A126" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B126" s="1">
@@ -10387,7 +10586,7 @@
       </c>
     </row>
     <row r="127" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A127" s="14" t="s">
+      <c r="A127" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="4">
@@ -10417,13 +10616,13 @@
       <c r="J127" s="4">
         <v>9</v>
       </c>
-      <c r="K127" s="16">
+      <c r="K127" s="15">
         <v>10</v>
       </c>
       <c r="L127" s="4">
         <v>11</v>
       </c>
-      <c r="M127" s="16">
+      <c r="M127" s="15">
         <v>12</v>
       </c>
       <c r="N127" s="4">
@@ -10432,7 +10631,7 @@
       <c r="O127" s="4">
         <v>14</v>
       </c>
-      <c r="P127" s="16">
+      <c r="P127" s="15">
         <v>15</v>
       </c>
       <c r="Q127" s="4">
@@ -10441,7 +10640,7 @@
       <c r="R127" s="4">
         <v>17</v>
       </c>
-      <c r="S127" s="16">
+      <c r="S127" s="15">
         <v>18</v>
       </c>
       <c r="T127" s="4">
@@ -10453,7 +10652,7 @@
       <c r="V127" s="4">
         <v>21</v>
       </c>
-      <c r="W127" s="16">
+      <c r="W127" s="15">
         <v>22</v>
       </c>
       <c r="X127" s="4">
@@ -10462,7 +10661,7 @@
       <c r="Y127" s="4">
         <v>24</v>
       </c>
-      <c r="Z127" s="16">
+      <c r="Z127" s="15">
         <v>25</v>
       </c>
     </row>
@@ -10483,15 +10682,15 @@
       <c r="Y128"/>
     </row>
     <row r="129" spans="1:27" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M129" s="15"/>
-      <c r="N129" s="15"/>
-      <c r="O129" s="15"/>
-      <c r="P129" s="15"/>
-      <c r="Q129" s="15"/>
-      <c r="R129" s="15"/>
-      <c r="S129" s="15"/>
-      <c r="T129" s="15"/>
-      <c r="U129" s="15"/>
+      <c r="M129" s="14"/>
+      <c r="N129" s="14"/>
+      <c r="O129" s="14"/>
+      <c r="P129" s="14"/>
+      <c r="Q129" s="14"/>
+      <c r="R129" s="14"/>
+      <c r="S129" s="14"/>
+      <c r="T129" s="14"/>
+      <c r="U129" s="14"/>
       <c r="W129"/>
       <c r="X129"/>
       <c r="Y129"/>
@@ -10502,31 +10701,31 @@
       <c r="Y130"/>
     </row>
     <row r="131" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B131" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-      <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
-      <c r="M131" s="8"/>
-      <c r="N131" s="8"/>
-      <c r="O131" s="8"/>
-      <c r="P131" s="8"/>
-      <c r="Q131" s="8"/>
-      <c r="R131" s="8"/>
-      <c r="S131" s="8"/>
-      <c r="T131" s="8"/>
-      <c r="U131" s="8"/>
-      <c r="V131" s="8"/>
-      <c r="W131" s="8"/>
-      <c r="X131" s="8"/>
+      <c r="B131" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="34"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="34"/>
+      <c r="F131" s="34"/>
+      <c r="G131" s="34"/>
+      <c r="H131" s="34"/>
+      <c r="I131" s="34"/>
+      <c r="J131" s="34"/>
+      <c r="K131" s="34"/>
+      <c r="L131" s="34"/>
+      <c r="M131" s="34"/>
+      <c r="N131" s="34"/>
+      <c r="O131" s="34"/>
+      <c r="P131" s="34"/>
+      <c r="Q131" s="34"/>
+      <c r="R131" s="34"/>
+      <c r="S131" s="34"/>
+      <c r="T131" s="34"/>
+      <c r="U131" s="34"/>
+      <c r="V131" s="34"/>
+      <c r="W131" s="34"/>
+      <c r="X131" s="34"/>
       <c r="Y131"/>
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.25">
@@ -10553,8 +10752,8 @@
       <c r="T132" s="3"/>
       <c r="U132" s="3"/>
       <c r="V132" s="3"/>
-      <c r="W132" s="9"/>
-      <c r="X132" s="10"/>
+      <c r="W132" s="8"/>
+      <c r="X132" s="9"/>
       <c r="Y132"/>
     </row>
     <row r="133" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -13420,186 +13619,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="A1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
     </row>
     <row r="2" spans="1:27" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-    </row>
-    <row r="3" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="18"/>
+      <c r="A2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+    </row>
+    <row r="3" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="16"/>
     </row>
     <row r="4" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="19">
-        <v>1</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17">
         <v>4</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="17">
         <v>5</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>8</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="17">
         <v>12</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="17">
         <v>15</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="17">
         <v>16</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="17">
         <v>17</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="24">
         <v>6</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="25">
         <v>7</v>
       </c>
-      <c r="L4" s="27">
-        <v>2</v>
-      </c>
-      <c r="M4" s="27">
+      <c r="L4" s="25">
+        <v>2</v>
+      </c>
+      <c r="M4" s="25">
         <v>18</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="25">
         <v>19</v>
       </c>
-      <c r="O4" s="27">
+      <c r="O4" s="25">
         <v>14</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="26">
         <v>3</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="17">
         <v>21</v>
       </c>
-      <c r="R4" s="19">
+      <c r="R4" s="17">
         <v>22</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="17">
         <v>23</v>
       </c>
-      <c r="T4" s="26">
+      <c r="T4" s="24">
         <v>10</v>
       </c>
-      <c r="U4" s="27">
+      <c r="U4" s="25">
         <v>13</v>
       </c>
-      <c r="V4" s="27">
+      <c r="V4" s="25">
         <v>11</v>
       </c>
-      <c r="W4" s="27">
+      <c r="W4" s="25">
         <v>20</v>
       </c>
-      <c r="X4" s="27">
+      <c r="X4" s="25">
         <v>24</v>
       </c>
-      <c r="Y4" s="28">
+      <c r="Y4" s="26">
         <v>9</v>
       </c>
-      <c r="Z4" s="19">
+      <c r="Z4" s="17">
         <v>25</v>
       </c>
       <c r="AA4" s="4"/>
     </row>
     <row r="5" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A5" s="20">
+      <c r="A5" s="18">
         <v>1</v>
       </c>
       <c r="B5" s="1">
@@ -13626,25 +13825,25 @@
       <c r="I5" s="5">
         <v>-0.14692834634061069</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="27">
         <v>-9.8230575298086001E-2</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="28">
         <v>-0.16133327699994318</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="29">
         <v>-0.18214478965583</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="28">
         <v>-8.5987913709947128E-2</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="28">
         <v>-1.1361827159631528E-2</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="28">
         <v>-0.27476490915870477</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="30">
         <v>-8.8161202160043875E-2</v>
       </c>
       <c r="Q5" s="5">
@@ -13656,33 +13855,33 @@
       <c r="S5" s="5">
         <v>-4.1595243607084192E-2</v>
       </c>
-      <c r="T5" s="29">
+      <c r="T5" s="27">
         <v>6.4659755408774999E-2</v>
       </c>
-      <c r="U5" s="30">
+      <c r="U5" s="28">
         <v>4.9902682409816795E-2</v>
       </c>
-      <c r="V5" s="30">
+      <c r="V5" s="28">
         <v>0.11099863578608991</v>
       </c>
-      <c r="W5" s="30">
+      <c r="W5" s="28">
         <v>0.13656238722891059</v>
       </c>
-      <c r="X5" s="30">
+      <c r="X5" s="28">
         <v>0.22895154620379699</v>
       </c>
-      <c r="Y5" s="32">
+      <c r="Y5" s="30">
         <v>0.11031164095248254</v>
       </c>
       <c r="Z5" s="5">
         <v>-3.9056857259401501E-2</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="20">
+      <c r="A6" s="18">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -13709,25 +13908,25 @@
       <c r="I6" s="5">
         <v>-0.12822228165453411</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="27">
         <v>6.7914260728438064E-2</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="28">
         <v>-7.8465187820372581E-2</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="29">
         <v>4.3481161394546004E-2</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="28">
         <v>0.24225681116204989</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="28">
         <v>4.4837848968534266E-2</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="28">
         <v>4.9226423377449487E-2</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="30">
         <v>9.0354902517995009E-2</v>
       </c>
       <c r="Q6" s="5">
@@ -13739,33 +13938,33 @@
       <c r="S6" s="5">
         <v>7.5173293186625148E-2</v>
       </c>
-      <c r="T6" s="29">
+      <c r="T6" s="27">
         <v>-0.23669080045742036</v>
       </c>
-      <c r="U6" s="30">
+      <c r="U6" s="28">
         <v>-0.12720436057296586</v>
       </c>
-      <c r="V6" s="30">
+      <c r="V6" s="28">
         <v>-7.01428717975493E-2</v>
       </c>
-      <c r="W6" s="30">
+      <c r="W6" s="28">
         <v>-0.16563066050225134</v>
       </c>
-      <c r="X6" s="30">
+      <c r="X6" s="28">
         <v>-3.2959346998137296E-2</v>
       </c>
-      <c r="Y6" s="32">
+      <c r="Y6" s="30">
         <v>-1.2517730639381331E-3</v>
       </c>
       <c r="Z6" s="5">
         <v>-5.3596856596641269E-2</v>
       </c>
-      <c r="AA6" s="21">
+      <c r="AA6" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="18">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -13792,25 +13991,25 @@
       <c r="I7" s="5">
         <v>0.19508015865187464</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="27">
         <v>-2.11207317362316E-2</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="28">
         <v>0.13183885112665208</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="29">
         <v>0.10754335714866142</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="28">
         <v>-0.21867894524070053</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="28">
         <v>-0.11166383701469335</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="28">
         <v>-8.1334737140329738E-2</v>
       </c>
-      <c r="P7" s="32">
+      <c r="P7" s="30">
         <v>8.7115410911312557E-2</v>
       </c>
       <c r="Q7" s="5">
@@ -13822,33 +14021,33 @@
       <c r="S7" s="5">
         <v>0.10099468544210755</v>
       </c>
-      <c r="T7" s="29">
+      <c r="T7" s="27">
         <v>0.14502500441352792</v>
       </c>
-      <c r="U7" s="30">
+      <c r="U7" s="28">
         <v>0.11541975584565882</v>
       </c>
-      <c r="V7" s="30">
+      <c r="V7" s="28">
         <v>0.20649519651887238</v>
       </c>
-      <c r="W7" s="30">
+      <c r="W7" s="28">
         <v>0.16077693163343895</v>
       </c>
-      <c r="X7" s="30">
+      <c r="X7" s="28">
         <v>0.17970186541018943</v>
       </c>
-      <c r="Y7" s="32">
+      <c r="Y7" s="30">
         <v>2.3190144951251889E-2</v>
       </c>
       <c r="Z7" s="5">
         <v>0.26106198185287238</v>
       </c>
-      <c r="AA7" s="21">
+      <c r="AA7" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="18">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -13875,25 +14074,25 @@
       <c r="I8" s="5">
         <v>1.9723681573208564E-2</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="27">
         <v>0.15352602971951751</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="28">
         <v>1.922497056300021E-2</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="29">
         <v>-0.10360906535666387</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="28">
         <v>-3.1870858785940169E-2</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="28">
         <v>-0.2912054877170282</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="28">
         <v>-5.7926772692687492E-2</v>
       </c>
-      <c r="P8" s="32">
+      <c r="P8" s="30">
         <v>-9.7165773500034525E-2</v>
       </c>
       <c r="Q8" s="5">
@@ -13905,33 +14104,33 @@
       <c r="S8" s="5">
         <v>0.19341862011907732</v>
       </c>
-      <c r="T8" s="29">
+      <c r="T8" s="27">
         <v>2.3829140851003613E-2</v>
       </c>
-      <c r="U8" s="30">
+      <c r="U8" s="28">
         <v>-6.975638473724767E-3</v>
       </c>
-      <c r="V8" s="30">
+      <c r="V8" s="28">
         <v>0.18821312498082488</v>
       </c>
-      <c r="W8" s="30">
+      <c r="W8" s="28">
         <v>8.6684123033595517E-2</v>
       </c>
-      <c r="X8" s="30">
+      <c r="X8" s="28">
         <v>0.25666932971464768</v>
       </c>
-      <c r="Y8" s="32">
+      <c r="Y8" s="30">
         <v>0.35359573766636215</v>
       </c>
       <c r="Z8" s="5">
         <v>-2.7711955959579735E-2</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="AA8" s="19">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="18">
         <v>12</v>
       </c>
       <c r="B9" s="1">
@@ -13958,25 +14157,25 @@
       <c r="I9" s="5">
         <v>-0.3899035770872446</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="27">
         <v>-0.13487592732820733</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="28">
         <v>-5.086780989479369E-2</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="29">
         <v>-6.2432447279098906E-2</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="28">
         <v>3.2846916273464644E-2</v>
       </c>
-      <c r="N9" s="30">
+      <c r="N9" s="28">
         <v>-3.1062221113246732E-2</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="28">
         <v>0.3490647378327969</v>
       </c>
-      <c r="P9" s="32">
+      <c r="P9" s="30">
         <v>0.13312456211023102</v>
       </c>
       <c r="Q9" s="5">
@@ -13988,33 +14187,33 @@
       <c r="S9" s="5">
         <v>0.1170522345441356</v>
       </c>
-      <c r="T9" s="29">
+      <c r="T9" s="27">
         <v>4.6562410464525063E-2</v>
       </c>
-      <c r="U9" s="30">
+      <c r="U9" s="28">
         <v>-2.3335663681629842E-2</v>
       </c>
-      <c r="V9" s="30">
+      <c r="V9" s="28">
         <v>-0.11988613400536688</v>
       </c>
-      <c r="W9" s="30">
+      <c r="W9" s="28">
         <v>-6.9811238865750075E-3</v>
       </c>
-      <c r="X9" s="30">
+      <c r="X9" s="28">
         <v>8.291082445887131E-2</v>
       </c>
-      <c r="Y9" s="32">
+      <c r="Y9" s="30">
         <v>-3.7824488634140847E-2</v>
       </c>
       <c r="Z9" s="5">
         <v>-3.6695747298216418E-2</v>
       </c>
-      <c r="AA9" s="21">
+      <c r="AA9" s="19">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+      <c r="A10" s="18">
         <v>15</v>
       </c>
       <c r="B10" s="1">
@@ -14041,25 +14240,25 @@
       <c r="I10" s="5">
         <v>-8.8732195170677555E-2</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="27">
         <v>9.7020639301301878E-2</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="28">
         <v>-6.3052511031610511E-2</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="29">
         <v>8.2448009128863006E-2</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="28">
         <v>0.15311755351276363</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="28">
         <v>-2.8897545230377266E-2</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="28">
         <v>0.17594960459177295</v>
       </c>
-      <c r="P10" s="32">
+      <c r="P10" s="30">
         <v>-7.4784883205154681E-2</v>
       </c>
       <c r="Q10" s="5">
@@ -14071,33 +14270,33 @@
       <c r="S10" s="5">
         <v>0.10568928011285003</v>
       </c>
-      <c r="T10" s="29">
+      <c r="T10" s="27">
         <v>-0.11264260992621762</v>
       </c>
-      <c r="U10" s="30">
+      <c r="U10" s="28">
         <v>-0.13106068773519017</v>
       </c>
-      <c r="V10" s="30">
+      <c r="V10" s="28">
         <v>-0.1327450400459651</v>
       </c>
-      <c r="W10" s="30">
+      <c r="W10" s="28">
         <v>-0.21845639140154974</v>
       </c>
-      <c r="X10" s="30">
+      <c r="X10" s="28">
         <v>-3.6742029591663432E-3</v>
       </c>
-      <c r="Y10" s="32">
+      <c r="Y10" s="30">
         <v>4.0865037190951588E-2</v>
       </c>
       <c r="Z10" s="5">
         <v>-0.25403953652950756</v>
       </c>
-      <c r="AA10" s="21">
+      <c r="AA10" s="19">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="18">
         <v>16</v>
       </c>
       <c r="B11" s="1">
@@ -14124,25 +14323,25 @@
       <c r="I11" s="5">
         <v>-7.7900395209908962E-2</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="27">
         <v>3.2216440613423887E-2</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="28">
         <v>1.3062510584705197E-2</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="29">
         <v>-4.9900695886495219E-2</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="28">
         <v>-2.2405242798754707E-2</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="28">
         <v>-4.5543795720906208E-2</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="28">
         <v>-0.1202225760656362</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="30">
         <v>-3.0787456944791836E-2</v>
       </c>
       <c r="Q11" s="5">
@@ -14154,33 +14353,33 @@
       <c r="S11" s="5">
         <v>4.5582014297170393E-3</v>
       </c>
-      <c r="T11" s="29">
+      <c r="T11" s="27">
         <v>-5.7426047417467381E-2</v>
       </c>
-      <c r="U11" s="30">
+      <c r="U11" s="28">
         <v>-3.477296876272179E-2</v>
       </c>
-      <c r="V11" s="30">
+      <c r="V11" s="28">
         <v>-1.9931019865757505E-2</v>
       </c>
-      <c r="W11" s="30">
+      <c r="W11" s="28">
         <v>-2.6591571301047062E-3</v>
       </c>
-      <c r="X11" s="30">
+      <c r="X11" s="28">
         <v>2.4839623285128322E-2</v>
       </c>
-      <c r="Y11" s="32">
+      <c r="Y11" s="30">
         <v>0.10796827700400775</v>
       </c>
       <c r="Z11" s="5">
         <v>-0.25414541824091613</v>
       </c>
-      <c r="AA11" s="21">
+      <c r="AA11" s="19">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
+      <c r="A12" s="18">
         <v>17</v>
       </c>
       <c r="B12" s="1">
@@ -14207,25 +14406,25 @@
       <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="27">
         <v>8.6253822598997998E-2</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="28">
         <v>0.15181622313790993</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="29">
         <v>0.11525634482406223</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="28">
         <v>-2.4998759449622071E-2</v>
       </c>
-      <c r="N12" s="30">
+      <c r="N12" s="28">
         <v>-0.12010450393608642</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="28">
         <v>-0.15075781262368698</v>
       </c>
-      <c r="P12" s="32">
+      <c r="P12" s="30">
         <v>-0.14687611507109388</v>
       </c>
       <c r="Q12" s="5">
@@ -14237,33 +14436,33 @@
       <c r="S12" s="5">
         <v>7.5642153572622869E-2</v>
       </c>
-      <c r="T12" s="29">
+      <c r="T12" s="27">
         <v>-2.6504683508668209E-2</v>
       </c>
-      <c r="U12" s="30">
+      <c r="U12" s="28">
         <v>0.19374919871666663</v>
       </c>
-      <c r="V12" s="30">
+      <c r="V12" s="28">
         <v>0.22851600231347036</v>
       </c>
-      <c r="W12" s="30">
+      <c r="W12" s="28">
         <v>-3.7096984880948057E-2</v>
       </c>
-      <c r="X12" s="30">
+      <c r="X12" s="28">
         <v>3.3342494837538962E-2</v>
       </c>
-      <c r="Y12" s="32">
+      <c r="Y12" s="30">
         <v>-5.1146668675823605E-3</v>
       </c>
       <c r="Z12" s="5">
         <v>0.24856289411024246</v>
       </c>
-      <c r="AA12" s="21">
+      <c r="AA12" s="19">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="18">
         <v>6</v>
       </c>
       <c r="B13" s="1">
@@ -14290,25 +14489,25 @@
       <c r="I13" s="5">
         <v>8.6253822598997998E-2</v>
       </c>
-      <c r="J13" s="29">
-        <v>1</v>
-      </c>
-      <c r="K13" s="30">
+      <c r="J13" s="27">
+        <v>1</v>
+      </c>
+      <c r="K13" s="28">
         <v>0.435635278345685</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="29">
         <v>0.39528747038765844</v>
       </c>
-      <c r="M13" s="30">
+      <c r="M13" s="28">
         <v>0.32059792249553865</v>
       </c>
-      <c r="N13" s="30">
+      <c r="N13" s="28">
         <v>0.28139255579091083</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="28">
         <v>0.12478417128398646</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P13" s="30">
         <v>0.33076189781928195</v>
       </c>
       <c r="Q13" s="5">
@@ -14320,33 +14519,33 @@
       <c r="S13" s="5">
         <v>-0.1307784670802481</v>
       </c>
-      <c r="T13" s="29">
+      <c r="T13" s="27">
         <v>-0.32840138427998289</v>
       </c>
-      <c r="U13" s="30">
+      <c r="U13" s="28">
         <v>-0.35480375582832596</v>
       </c>
-      <c r="V13" s="30">
+      <c r="V13" s="28">
         <v>-0.17698170509936423</v>
       </c>
-      <c r="W13" s="30">
+      <c r="W13" s="28">
         <v>-0.25375583998261037</v>
       </c>
-      <c r="X13" s="30">
+      <c r="X13" s="28">
         <v>-0.3299041945864789</v>
       </c>
-      <c r="Y13" s="32">
+      <c r="Y13" s="30">
         <v>-0.25079739520044575</v>
       </c>
       <c r="Z13" s="5">
         <v>7.856156257298888E-2</v>
       </c>
-      <c r="AA13" s="21">
+      <c r="AA13" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A14" s="20">
+      <c r="A14" s="18">
         <v>7</v>
       </c>
       <c r="B14" s="1">
@@ -14373,25 +14572,25 @@
       <c r="I14" s="5">
         <v>0.15181622313790993</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="27">
         <v>0.435635278345685</v>
       </c>
-      <c r="K14" s="30">
-        <v>1</v>
-      </c>
-      <c r="L14" s="31">
+      <c r="K14" s="28">
+        <v>1</v>
+      </c>
+      <c r="L14" s="29">
         <v>0.49629293421679155</v>
       </c>
-      <c r="M14" s="30">
+      <c r="M14" s="28">
         <v>0.28249723186560727</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="28">
         <v>0.3210966622440013</v>
       </c>
-      <c r="O14" s="30">
+      <c r="O14" s="28">
         <v>0.24249511657187131</v>
       </c>
-      <c r="P14" s="32">
+      <c r="P14" s="30">
         <v>0.26225569843282864</v>
       </c>
       <c r="Q14" s="5">
@@ -14403,33 +14602,33 @@
       <c r="S14" s="5">
         <v>-0.20142321338486413</v>
       </c>
-      <c r="T14" s="29">
+      <c r="T14" s="27">
         <v>-0.21489400963115349</v>
       </c>
-      <c r="U14" s="30">
+      <c r="U14" s="28">
         <v>-0.28682752740633899</v>
       </c>
-      <c r="V14" s="30">
+      <c r="V14" s="28">
         <v>-0.22777696841973272</v>
       </c>
-      <c r="W14" s="30">
+      <c r="W14" s="28">
         <v>-0.20130738682806631</v>
       </c>
-      <c r="X14" s="30">
+      <c r="X14" s="28">
         <v>-0.33786539992541892</v>
       </c>
-      <c r="Y14" s="32">
+      <c r="Y14" s="30">
         <v>-0.39405789991326584</v>
       </c>
       <c r="Z14" s="5">
         <v>0.16127335014570013</v>
       </c>
-      <c r="AA14" s="21">
+      <c r="AA14" s="19">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A15" s="20">
+      <c r="A15" s="18">
         <v>2</v>
       </c>
       <c r="B15" s="1">
@@ -14456,25 +14655,25 @@
       <c r="I15" s="5">
         <v>0.11525634482406223</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="27">
         <v>0.39528747038765844</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="28">
         <v>0.49629293421679155</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="29">
         <v>0.99999999999999989</v>
       </c>
-      <c r="M15" s="30">
+      <c r="M15" s="28">
         <v>0.43828004006829052</v>
       </c>
-      <c r="N15" s="30">
+      <c r="N15" s="28">
         <v>0.43026299315783689</v>
       </c>
-      <c r="O15" s="30">
+      <c r="O15" s="28">
         <v>0.36559744351653112</v>
       </c>
-      <c r="P15" s="32">
+      <c r="P15" s="30">
         <v>0.32681488788479279</v>
       </c>
       <c r="Q15" s="5">
@@ -14486,33 +14685,33 @@
       <c r="S15" s="5">
         <v>-7.4398212107182879E-2</v>
       </c>
-      <c r="T15" s="29">
+      <c r="T15" s="27">
         <v>-0.34379641539660116</v>
       </c>
-      <c r="U15" s="30">
+      <c r="U15" s="28">
         <v>-0.34257846731855968</v>
       </c>
-      <c r="V15" s="30">
+      <c r="V15" s="28">
         <v>-0.40202952232214195</v>
       </c>
-      <c r="W15" s="30">
+      <c r="W15" s="28">
         <v>-0.33841391330336296</v>
       </c>
-      <c r="X15" s="30">
+      <c r="X15" s="28">
         <v>-0.501473079312028</v>
       </c>
-      <c r="Y15" s="32">
+      <c r="Y15" s="30">
         <v>-0.38087950786795938</v>
       </c>
       <c r="Z15" s="5">
         <v>4.7374962626922056E-2</v>
       </c>
-      <c r="AA15" s="21">
+      <c r="AA15" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A16" s="20">
+      <c r="A16" s="18">
         <v>18</v>
       </c>
       <c r="B16" s="1">
@@ -14539,25 +14738,25 @@
       <c r="I16" s="5">
         <v>-2.4998759449622071E-2</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="27">
         <v>0.32059792249553865</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="28">
         <v>0.28249723186560727</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="29">
         <v>0.43828004006829052</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="28">
         <v>0.99999999999999978</v>
       </c>
-      <c r="N16" s="30">
+      <c r="N16" s="28">
         <v>0.46931595969871104</v>
       </c>
-      <c r="O16" s="30">
+      <c r="O16" s="28">
         <v>0.33731725360387321</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="30">
         <v>0.26976350050712733</v>
       </c>
       <c r="Q16" s="5">
@@ -14569,33 +14768,33 @@
       <c r="S16" s="5">
         <v>-7.802108773361062E-2</v>
       </c>
-      <c r="T16" s="29">
+      <c r="T16" s="27">
         <v>-0.54334449432543219</v>
       </c>
-      <c r="U16" s="30">
+      <c r="U16" s="28">
         <v>-0.46843331784468556</v>
       </c>
-      <c r="V16" s="30">
+      <c r="V16" s="28">
         <v>-0.36991009953442228</v>
       </c>
-      <c r="W16" s="30">
+      <c r="W16" s="28">
         <v>-0.47313808691311676</v>
       </c>
-      <c r="X16" s="30">
+      <c r="X16" s="28">
         <v>-0.50991653408828075</v>
       </c>
-      <c r="Y16" s="32">
+      <c r="Y16" s="30">
         <v>-0.27785148556861033</v>
       </c>
       <c r="Z16" s="5">
         <v>-3.2756471647741835E-2</v>
       </c>
-      <c r="AA16" s="21">
+      <c r="AA16" s="19">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
+      <c r="A17" s="18">
         <v>19</v>
       </c>
       <c r="B17" s="1">
@@ -14622,25 +14821,25 @@
       <c r="I17" s="5">
         <v>-0.12010450393608642</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="27">
         <v>0.28139255579091083</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="28">
         <v>0.3210966622440013</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="29">
         <v>0.43026299315783689</v>
       </c>
-      <c r="M17" s="30">
+      <c r="M17" s="28">
         <v>0.46931595969871104</v>
       </c>
-      <c r="N17" s="30">
+      <c r="N17" s="28">
         <v>0.99999999999999989</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="28">
         <v>0.36771073991190234</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="30">
         <v>0.34277718484949499</v>
       </c>
       <c r="Q17" s="5">
@@ -14652,33 +14851,33 @@
       <c r="S17" s="5">
         <v>-0.22079406843313398</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T17" s="27">
         <v>-0.27402201796647907</v>
       </c>
-      <c r="U17" s="30">
+      <c r="U17" s="28">
         <v>-0.40036582520398439</v>
       </c>
-      <c r="V17" s="30">
+      <c r="V17" s="28">
         <v>-0.44309243533034198</v>
       </c>
-      <c r="W17" s="30">
+      <c r="W17" s="28">
         <v>-0.34296076845262818</v>
       </c>
-      <c r="X17" s="30">
+      <c r="X17" s="28">
         <v>-0.66417254053371766</v>
       </c>
-      <c r="Y17" s="32">
+      <c r="Y17" s="30">
         <v>-0.42761920743098453</v>
       </c>
       <c r="Z17" s="5">
         <v>-1.8726352412337069E-2</v>
       </c>
-      <c r="AA17" s="21">
+      <c r="AA17" s="19">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="A18" s="18">
         <v>14</v>
       </c>
       <c r="B18" s="1">
@@ -14705,25 +14904,25 @@
       <c r="I18" s="5">
         <v>-0.15075781262368698</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="27">
         <v>0.12478417128398646</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="28">
         <v>0.24249511657187131</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="29">
         <v>0.36559744351653112</v>
       </c>
-      <c r="M18" s="30">
+      <c r="M18" s="28">
         <v>0.33731725360387321</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="28">
         <v>0.36771073991190234</v>
       </c>
-      <c r="O18" s="30">
-        <v>1</v>
-      </c>
-      <c r="P18" s="32">
+      <c r="O18" s="28">
+        <v>1</v>
+      </c>
+      <c r="P18" s="30">
         <v>0.48711364142635638</v>
       </c>
       <c r="Q18" s="5">
@@ -14735,33 +14934,33 @@
       <c r="S18" s="5">
         <v>-4.2583461903490001E-2</v>
       </c>
-      <c r="T18" s="29">
+      <c r="T18" s="27">
         <v>-0.14760989343415931</v>
       </c>
-      <c r="U18" s="30">
+      <c r="U18" s="28">
         <v>-0.23493789356007458</v>
       </c>
-      <c r="V18" s="30">
+      <c r="V18" s="28">
         <v>-0.39318826593373002</v>
       </c>
-      <c r="W18" s="30">
+      <c r="W18" s="28">
         <v>-0.37947688952557662</v>
       </c>
-      <c r="X18" s="30">
+      <c r="X18" s="28">
         <v>-0.32438682433003219</v>
       </c>
-      <c r="Y18" s="32">
+      <c r="Y18" s="30">
         <v>-0.21664709178461342</v>
       </c>
       <c r="Z18" s="5">
         <v>0.10362596419666328</v>
       </c>
-      <c r="AA18" s="21">
+      <c r="AA18" s="19">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
+      <c r="A19" s="18">
         <v>3</v>
       </c>
       <c r="B19" s="1">
@@ -14788,25 +14987,25 @@
       <c r="I19" s="5">
         <v>-0.14687611507109388</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="27">
         <v>0.33076189781928195</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="28">
         <v>0.26225569843282864</v>
       </c>
-      <c r="L19" s="31">
+      <c r="L19" s="29">
         <v>0.32681488788479279</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="28">
         <v>0.26976350050712733</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="28">
         <v>0.34277718484949499</v>
       </c>
-      <c r="O19" s="30">
+      <c r="O19" s="28">
         <v>0.48711364142635638</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="30">
         <v>0.99999999999999989</v>
       </c>
       <c r="Q19" s="5">
@@ -14818,33 +15017,33 @@
       <c r="S19" s="5">
         <v>-0.1594971629105523</v>
       </c>
-      <c r="T19" s="29">
+      <c r="T19" s="27">
         <v>-0.11831038346218617</v>
       </c>
-      <c r="U19" s="30">
+      <c r="U19" s="28">
         <v>-0.12847939377783699</v>
       </c>
-      <c r="V19" s="30">
+      <c r="V19" s="28">
         <v>-0.27997827679861809</v>
       </c>
-      <c r="W19" s="30">
+      <c r="W19" s="28">
         <v>-0.1338774919170567</v>
       </c>
-      <c r="X19" s="30">
+      <c r="X19" s="28">
         <v>-0.24189149861542253</v>
       </c>
-      <c r="Y19" s="32">
+      <c r="Y19" s="30">
         <v>-0.25919202860050572</v>
       </c>
       <c r="Z19" s="5">
         <v>7.9083987564663671E-2</v>
       </c>
-      <c r="AA19" s="21">
+      <c r="AA19" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
+      <c r="A20" s="18">
         <v>21</v>
       </c>
       <c r="B20" s="1">
@@ -14871,25 +15070,25 @@
       <c r="I20" s="5">
         <v>9.7986830326500282E-2</v>
       </c>
-      <c r="J20" s="29">
+      <c r="J20" s="27">
         <v>0.15846160386148589</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="28">
         <v>0.15443790350888018</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="29">
         <v>0.24070917077214463</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="28">
         <v>8.324227726881181E-2</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="28">
         <v>0.15834434406291359</v>
       </c>
-      <c r="O20" s="30">
+      <c r="O20" s="28">
         <v>0.33584987473394107</v>
       </c>
-      <c r="P20" s="32">
+      <c r="P20" s="30">
         <v>0.20294337298344189</v>
       </c>
       <c r="Q20" s="5">
@@ -14901,33 +15100,33 @@
       <c r="S20" s="5">
         <v>0.13783988829047064</v>
       </c>
-      <c r="T20" s="29">
+      <c r="T20" s="27">
         <v>-5.2594707940487033E-2</v>
       </c>
-      <c r="U20" s="30">
+      <c r="U20" s="28">
         <v>-0.15031007779924754</v>
       </c>
-      <c r="V20" s="30">
+      <c r="V20" s="28">
         <v>-6.5824740378209526E-2</v>
       </c>
-      <c r="W20" s="30">
+      <c r="W20" s="28">
         <v>-0.12141072479661207</v>
       </c>
-      <c r="X20" s="30">
+      <c r="X20" s="28">
         <v>-7.242550145145131E-2</v>
       </c>
-      <c r="Y20" s="32">
+      <c r="Y20" s="30">
         <v>-0.15730394904327399</v>
       </c>
       <c r="Z20" s="5">
         <v>0.19282430566250197</v>
       </c>
-      <c r="AA20" s="21">
+      <c r="AA20" s="19">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A21" s="20">
+      <c r="A21" s="18">
         <v>22</v>
       </c>
       <c r="B21" s="1">
@@ -14954,25 +15153,25 @@
       <c r="I21" s="5">
         <v>-4.7076002883888621E-2</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="27">
         <v>0.15387787645682835</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="28">
         <v>8.314277466738125E-2</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="29">
         <v>7.8059244842096046E-2</v>
       </c>
-      <c r="M21" s="30">
+      <c r="M21" s="28">
         <v>8.9911919363836565E-2</v>
       </c>
-      <c r="N21" s="30">
+      <c r="N21" s="28">
         <v>0.10679876830063741</v>
       </c>
-      <c r="O21" s="30">
+      <c r="O21" s="28">
         <v>0.2709898728404172</v>
       </c>
-      <c r="P21" s="32">
+      <c r="P21" s="30">
         <v>0.13166978362072321</v>
       </c>
       <c r="Q21" s="5">
@@ -14984,33 +15183,33 @@
       <c r="S21" s="5">
         <v>0.19073081464409156</v>
       </c>
-      <c r="T21" s="29">
+      <c r="T21" s="27">
         <v>-5.0078246882594095E-2</v>
       </c>
-      <c r="U21" s="30">
+      <c r="U21" s="28">
         <v>-0.18884957840941466</v>
       </c>
-      <c r="V21" s="30">
+      <c r="V21" s="28">
         <v>-0.14991878200683179</v>
       </c>
-      <c r="W21" s="30">
+      <c r="W21" s="28">
         <v>-1.78639424256299E-2</v>
       </c>
-      <c r="X21" s="30">
+      <c r="X21" s="28">
         <v>-1.3476343302516819E-2</v>
       </c>
-      <c r="Y21" s="32">
+      <c r="Y21" s="30">
         <v>-3.108177046425066E-2</v>
       </c>
       <c r="Z21" s="5">
         <v>0.31851026312940606</v>
       </c>
-      <c r="AA21" s="21">
+      <c r="AA21" s="19">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
+      <c r="A22" s="18">
         <v>23</v>
       </c>
       <c r="B22" s="1">
@@ -15037,25 +15236,25 @@
       <c r="I22" s="5">
         <v>7.5642153572622869E-2</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="27">
         <v>-0.1307784670802481</v>
       </c>
-      <c r="K22" s="30">
+      <c r="K22" s="28">
         <v>-0.20142321338486413</v>
       </c>
-      <c r="L22" s="31">
+      <c r="L22" s="29">
         <v>-7.4398212107182879E-2</v>
       </c>
-      <c r="M22" s="30">
+      <c r="M22" s="28">
         <v>-7.802108773361062E-2</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="28">
         <v>-0.22079406843313398</v>
       </c>
-      <c r="O22" s="30">
+      <c r="O22" s="28">
         <v>-4.2583461903490001E-2</v>
       </c>
-      <c r="P22" s="32">
+      <c r="P22" s="30">
         <v>-0.1594971629105523</v>
       </c>
       <c r="Q22" s="5">
@@ -15067,33 +15266,33 @@
       <c r="S22" s="5">
         <v>1</v>
       </c>
-      <c r="T22" s="29">
+      <c r="T22" s="27">
         <v>8.3908361699164852E-2</v>
       </c>
-      <c r="U22" s="30">
+      <c r="U22" s="28">
         <v>0.13395357421020626</v>
       </c>
-      <c r="V22" s="30">
+      <c r="V22" s="28">
         <v>0.25242989360897039</v>
       </c>
-      <c r="W22" s="30">
+      <c r="W22" s="28">
         <v>3.7453500981410752E-2</v>
       </c>
-      <c r="X22" s="30">
+      <c r="X22" s="28">
         <v>0.2473522710101016</v>
       </c>
-      <c r="Y22" s="32">
+      <c r="Y22" s="30">
         <v>0.29786310577687403</v>
       </c>
       <c r="Z22" s="5">
         <v>0.16027705649014895</v>
       </c>
-      <c r="AA22" s="21">
+      <c r="AA22" s="19">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
+      <c r="A23" s="18">
         <v>10</v>
       </c>
       <c r="B23" s="1">
@@ -15120,25 +15319,25 @@
       <c r="I23" s="5">
         <v>-2.6504683508668209E-2</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="27">
         <v>-0.32840138427998289</v>
       </c>
-      <c r="K23" s="30">
+      <c r="K23" s="28">
         <v>-0.21489400963115349</v>
       </c>
-      <c r="L23" s="31">
+      <c r="L23" s="29">
         <v>-0.34379641539660116</v>
       </c>
-      <c r="M23" s="30">
+      <c r="M23" s="28">
         <v>-0.54334449432543219</v>
       </c>
-      <c r="N23" s="30">
+      <c r="N23" s="28">
         <v>-0.27402201796647907</v>
       </c>
-      <c r="O23" s="30">
+      <c r="O23" s="28">
         <v>-0.14760989343415931</v>
       </c>
-      <c r="P23" s="32">
+      <c r="P23" s="30">
         <v>-0.11831038346218617</v>
       </c>
       <c r="Q23" s="5">
@@ -15150,33 +15349,33 @@
       <c r="S23" s="5">
         <v>8.3908361699164852E-2</v>
       </c>
-      <c r="T23" s="29">
-        <v>1</v>
-      </c>
-      <c r="U23" s="30">
+      <c r="T23" s="27">
+        <v>1</v>
+      </c>
+      <c r="U23" s="28">
         <v>0.35211264681383642</v>
       </c>
-      <c r="V23" s="30">
+      <c r="V23" s="28">
         <v>0.27446702495223202</v>
       </c>
-      <c r="W23" s="30">
+      <c r="W23" s="28">
         <v>0.31555364576029138</v>
       </c>
-      <c r="X23" s="30">
+      <c r="X23" s="28">
         <v>0.32430558997518183</v>
       </c>
-      <c r="Y23" s="32">
+      <c r="Y23" s="30">
         <v>0.19306635240865708</v>
       </c>
       <c r="Z23" s="5">
         <v>4.2388778300499448E-3</v>
       </c>
-      <c r="AA23" s="21">
+      <c r="AA23" s="19">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+      <c r="A24" s="18">
         <v>13</v>
       </c>
       <c r="B24" s="1">
@@ -15203,25 +15402,25 @@
       <c r="I24" s="5">
         <v>0.19374919871666663</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="27">
         <v>-0.35480375582832596</v>
       </c>
-      <c r="K24" s="30">
+      <c r="K24" s="28">
         <v>-0.28682752740633899</v>
       </c>
-      <c r="L24" s="31">
+      <c r="L24" s="29">
         <v>-0.34257846731855968</v>
       </c>
-      <c r="M24" s="30">
+      <c r="M24" s="28">
         <v>-0.46843331784468556</v>
       </c>
-      <c r="N24" s="30">
+      <c r="N24" s="28">
         <v>-0.40036582520398439</v>
       </c>
-      <c r="O24" s="30">
+      <c r="O24" s="28">
         <v>-0.23493789356007458</v>
       </c>
-      <c r="P24" s="32">
+      <c r="P24" s="30">
         <v>-0.12847939377783699</v>
       </c>
       <c r="Q24" s="5">
@@ -15233,33 +15432,33 @@
       <c r="S24" s="5">
         <v>0.13395357421020626</v>
       </c>
-      <c r="T24" s="29">
+      <c r="T24" s="27">
         <v>0.35211264681383642</v>
       </c>
-      <c r="U24" s="30">
-        <v>1</v>
-      </c>
-      <c r="V24" s="30">
+      <c r="U24" s="28">
+        <v>1</v>
+      </c>
+      <c r="V24" s="28">
         <v>0.46045308844856297</v>
       </c>
-      <c r="W24" s="30">
+      <c r="W24" s="28">
         <v>0.31990406601702359</v>
       </c>
-      <c r="X24" s="30">
+      <c r="X24" s="28">
         <v>0.352014065592679</v>
       </c>
-      <c r="Y24" s="32">
+      <c r="Y24" s="30">
         <v>0.33675875123869548</v>
       </c>
       <c r="Z24" s="5">
         <v>8.2488347492546285E-2</v>
       </c>
-      <c r="AA24" s="21">
+      <c r="AA24" s="19">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
+      <c r="A25" s="18">
         <v>11</v>
       </c>
       <c r="B25" s="1">
@@ -15286,25 +15485,25 @@
       <c r="I25" s="5">
         <v>0.22851600231347036</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="27">
         <v>-0.17698170509936423</v>
       </c>
-      <c r="K25" s="30">
+      <c r="K25" s="28">
         <v>-0.22777696841973272</v>
       </c>
-      <c r="L25" s="31">
+      <c r="L25" s="29">
         <v>-0.40202952232214195</v>
       </c>
-      <c r="M25" s="30">
+      <c r="M25" s="28">
         <v>-0.36991009953442228</v>
       </c>
-      <c r="N25" s="30">
+      <c r="N25" s="28">
         <v>-0.44309243533034198</v>
       </c>
-      <c r="O25" s="30">
+      <c r="O25" s="28">
         <v>-0.39318826593373002</v>
       </c>
-      <c r="P25" s="32">
+      <c r="P25" s="30">
         <v>-0.27997827679861809</v>
       </c>
       <c r="Q25" s="5">
@@ -15316,33 +15515,33 @@
       <c r="S25" s="5">
         <v>0.25242989360897039</v>
       </c>
-      <c r="T25" s="29">
+      <c r="T25" s="27">
         <v>0.27446702495223202</v>
       </c>
-      <c r="U25" s="30">
+      <c r="U25" s="28">
         <v>0.46045308844856297</v>
       </c>
-      <c r="V25" s="30">
+      <c r="V25" s="28">
         <v>0.99999999999999989</v>
       </c>
-      <c r="W25" s="30">
+      <c r="W25" s="28">
         <v>0.29113976233532995</v>
       </c>
-      <c r="X25" s="30">
+      <c r="X25" s="28">
         <v>0.47857455553513317</v>
       </c>
-      <c r="Y25" s="32">
+      <c r="Y25" s="30">
         <v>0.43574362924168752</v>
       </c>
       <c r="Z25" s="5">
         <v>0.1541661957274959</v>
       </c>
-      <c r="AA25" s="21">
+      <c r="AA25" s="19">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
+      <c r="A26" s="18">
         <v>20</v>
       </c>
       <c r="B26" s="1">
@@ -15369,25 +15568,25 @@
       <c r="I26" s="5">
         <v>-3.7096984880948057E-2</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="27">
         <v>-0.25375583998261037</v>
       </c>
-      <c r="K26" s="30">
+      <c r="K26" s="28">
         <v>-0.20130738682806631</v>
       </c>
-      <c r="L26" s="31">
+      <c r="L26" s="29">
         <v>-0.33841391330336296</v>
       </c>
-      <c r="M26" s="30">
+      <c r="M26" s="28">
         <v>-0.47313808691311676</v>
       </c>
-      <c r="N26" s="30">
+      <c r="N26" s="28">
         <v>-0.34296076845262818</v>
       </c>
-      <c r="O26" s="30">
+      <c r="O26" s="28">
         <v>-0.37947688952557662</v>
       </c>
-      <c r="P26" s="32">
+      <c r="P26" s="30">
         <v>-0.1338774919170567</v>
       </c>
       <c r="Q26" s="5">
@@ -15399,33 +15598,33 @@
       <c r="S26" s="5">
         <v>3.7453500981410752E-2</v>
       </c>
-      <c r="T26" s="29">
+      <c r="T26" s="27">
         <v>0.31555364576029138</v>
       </c>
-      <c r="U26" s="30">
+      <c r="U26" s="28">
         <v>0.31990406601702359</v>
       </c>
-      <c r="V26" s="30">
+      <c r="V26" s="28">
         <v>0.29113976233532995</v>
       </c>
-      <c r="W26" s="30">
+      <c r="W26" s="28">
         <v>1.0000000000000002</v>
       </c>
-      <c r="X26" s="30">
+      <c r="X26" s="28">
         <v>0.41320758134531738</v>
       </c>
-      <c r="Y26" s="32">
+      <c r="Y26" s="30">
         <v>0.20987013413071887</v>
       </c>
       <c r="Z26" s="5">
         <v>3.042863896605023E-2</v>
       </c>
-      <c r="AA26" s="21">
+      <c r="AA26" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
+      <c r="A27" s="18">
         <v>24</v>
       </c>
       <c r="B27" s="1">
@@ -15452,25 +15651,25 @@
       <c r="I27" s="5">
         <v>3.3342494837538962E-2</v>
       </c>
-      <c r="J27" s="29">
+      <c r="J27" s="27">
         <v>-0.3299041945864789</v>
       </c>
-      <c r="K27" s="30">
+      <c r="K27" s="28">
         <v>-0.33786539992541892</v>
       </c>
-      <c r="L27" s="31">
+      <c r="L27" s="29">
         <v>-0.501473079312028</v>
       </c>
-      <c r="M27" s="30">
+      <c r="M27" s="28">
         <v>-0.50991653408828075</v>
       </c>
-      <c r="N27" s="30">
+      <c r="N27" s="28">
         <v>-0.66417254053371766</v>
       </c>
-      <c r="O27" s="30">
+      <c r="O27" s="28">
         <v>-0.32438682433003219</v>
       </c>
-      <c r="P27" s="32">
+      <c r="P27" s="30">
         <v>-0.24189149861542253</v>
       </c>
       <c r="Q27" s="5">
@@ -15482,33 +15681,33 @@
       <c r="S27" s="5">
         <v>0.2473522710101016</v>
       </c>
-      <c r="T27" s="29">
+      <c r="T27" s="27">
         <v>0.32430558997518183</v>
       </c>
-      <c r="U27" s="30">
+      <c r="U27" s="28">
         <v>0.352014065592679</v>
       </c>
-      <c r="V27" s="30">
+      <c r="V27" s="28">
         <v>0.47857455553513317</v>
       </c>
-      <c r="W27" s="30">
+      <c r="W27" s="28">
         <v>0.41320758134531738</v>
       </c>
-      <c r="X27" s="30">
+      <c r="X27" s="28">
         <v>1.0000000000000002</v>
       </c>
-      <c r="Y27" s="32">
+      <c r="Y27" s="30">
         <v>0.39508540522783692</v>
       </c>
       <c r="Z27" s="5">
         <v>5.1932045663466458E-2</v>
       </c>
-      <c r="AA27" s="21">
+      <c r="AA27" s="19">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
+      <c r="A28" s="18">
         <v>9</v>
       </c>
       <c r="B28" s="1">
@@ -15535,25 +15734,25 @@
       <c r="I28" s="5">
         <v>-5.1146668675823605E-3</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="27">
         <v>-0.25079739520044575</v>
       </c>
-      <c r="K28" s="30">
+      <c r="K28" s="28">
         <v>-0.39405789991326584</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="29">
         <v>-0.38087950786795938</v>
       </c>
-      <c r="M28" s="30">
+      <c r="M28" s="28">
         <v>-0.27785148556861033</v>
       </c>
-      <c r="N28" s="30">
+      <c r="N28" s="28">
         <v>-0.42761920743098453</v>
       </c>
-      <c r="O28" s="30">
+      <c r="O28" s="28">
         <v>-0.21664709178461342</v>
       </c>
-      <c r="P28" s="32">
+      <c r="P28" s="30">
         <v>-0.25919202860050572</v>
       </c>
       <c r="Q28" s="5">
@@ -15565,33 +15764,33 @@
       <c r="S28" s="5">
         <v>0.29786310577687403</v>
       </c>
-      <c r="T28" s="29">
+      <c r="T28" s="27">
         <v>0.19306635240865708</v>
       </c>
-      <c r="U28" s="30">
+      <c r="U28" s="28">
         <v>0.33675875123869548</v>
       </c>
-      <c r="V28" s="30">
+      <c r="V28" s="28">
         <v>0.43574362924168752</v>
       </c>
-      <c r="W28" s="30">
+      <c r="W28" s="28">
         <v>0.20987013413071887</v>
       </c>
-      <c r="X28" s="30">
+      <c r="X28" s="28">
         <v>0.39508540522783692</v>
       </c>
-      <c r="Y28" s="32">
+      <c r="Y28" s="30">
         <v>1.0000000000000002</v>
       </c>
       <c r="Z28" s="5">
         <v>-0.11837006818957803</v>
       </c>
-      <c r="AA28" s="21">
+      <c r="AA28" s="19">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:27" ht="21" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="18">
         <v>25</v>
       </c>
       <c r="B29" s="1">
@@ -15618,25 +15817,25 @@
       <c r="I29" s="5">
         <v>0.24856289411024246</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="27">
         <v>7.856156257298888E-2</v>
       </c>
-      <c r="K29" s="30">
+      <c r="K29" s="28">
         <v>0.16127335014570013</v>
       </c>
-      <c r="L29" s="31">
+      <c r="L29" s="29">
         <v>4.7374962626922056E-2</v>
       </c>
-      <c r="M29" s="30">
+      <c r="M29" s="28">
         <v>-3.2756471647741835E-2</v>
       </c>
-      <c r="N29" s="30">
+      <c r="N29" s="28">
         <v>-1.8726352412337069E-2</v>
       </c>
-      <c r="O29" s="30">
+      <c r="O29" s="28">
         <v>0.10362596419666328</v>
       </c>
-      <c r="P29" s="32">
+      <c r="P29" s="30">
         <v>7.9083987564663671E-2</v>
       </c>
       <c r="Q29" s="5">
@@ -15648,122 +15847,122 @@
       <c r="S29" s="5">
         <v>0.16027705649014895</v>
       </c>
-      <c r="T29" s="29">
+      <c r="T29" s="27">
         <v>4.2388778300499448E-3</v>
       </c>
-      <c r="U29" s="30">
+      <c r="U29" s="28">
         <v>8.2488347492546285E-2</v>
       </c>
-      <c r="V29" s="30">
+      <c r="V29" s="28">
         <v>0.1541661957274959</v>
       </c>
-      <c r="W29" s="30">
+      <c r="W29" s="28">
         <v>3.042863896605023E-2</v>
       </c>
-      <c r="X29" s="30">
+      <c r="X29" s="28">
         <v>5.1932045663466458E-2</v>
       </c>
-      <c r="Y29" s="32">
+      <c r="Y29" s="30">
         <v>-0.11837006818957803</v>
       </c>
       <c r="Z29" s="5">
         <v>1</v>
       </c>
-      <c r="AA29" s="21">
+      <c r="AA29" s="19">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="19">
-        <v>1</v>
-      </c>
-      <c r="C30" s="19">
+      <c r="B30" s="17">
+        <v>1</v>
+      </c>
+      <c r="C30" s="17">
         <v>4</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="17">
         <v>5</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="17">
         <v>8</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="17">
         <v>12</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="17">
         <v>15</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="17">
         <v>16</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="17">
         <v>17</v>
       </c>
-      <c r="J30" s="26">
+      <c r="J30" s="24">
         <v>6</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="25">
         <v>7</v>
       </c>
-      <c r="L30" s="27">
-        <v>2</v>
-      </c>
-      <c r="M30" s="27">
+      <c r="L30" s="25">
+        <v>2</v>
+      </c>
+      <c r="M30" s="25">
         <v>18</v>
       </c>
-      <c r="N30" s="27">
+      <c r="N30" s="25">
         <v>19</v>
       </c>
-      <c r="O30" s="27">
+      <c r="O30" s="25">
         <v>14</v>
       </c>
-      <c r="P30" s="28">
+      <c r="P30" s="26">
         <v>3</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30" s="17">
         <v>21</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R30" s="17">
         <v>22</v>
       </c>
-      <c r="S30" s="19">
+      <c r="S30" s="17">
         <v>23</v>
       </c>
-      <c r="T30" s="26">
+      <c r="T30" s="24">
         <v>10</v>
       </c>
-      <c r="U30" s="27">
+      <c r="U30" s="25">
         <v>13</v>
       </c>
-      <c r="V30" s="27">
+      <c r="V30" s="25">
         <v>11</v>
       </c>
-      <c r="W30" s="27">
+      <c r="W30" s="25">
         <v>20</v>
       </c>
-      <c r="X30" s="27">
+      <c r="X30" s="25">
         <v>24</v>
       </c>
-      <c r="Y30" s="28">
+      <c r="Y30" s="26">
         <v>9</v>
       </c>
-      <c r="Z30" s="19">
+      <c r="Z30" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J31" s="33"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="35"/>
-      <c r="T31" s="33"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="35"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="33"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -15783,6 +15982,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
small improvements in questions.xls
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="26835" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="26835" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
   <si>
     <t>Положительная корреляция — на вопросы отвечают чаще одинаково. Отрицательная — чаще дают противоположные ответы. 0 — ответы никак не связаны. 1 — ответы в точности одинаковые</t>
   </si>
@@ -238,6 +238,363 @@
   </si>
   <si>
     <t>Номер вопроса</t>
+  </si>
+  <si>
+    <t>Александрова-Зорина Елизавета Борисовна</t>
+  </si>
+  <si>
+    <t>Аншаков Михаил Геннадьевич</t>
+  </si>
+  <si>
+    <t>Ашурков Владимир Львович</t>
+  </si>
+  <si>
+    <t>Бадыкова Фиалка Ахмадеевна</t>
+  </si>
+  <si>
+    <t>Бакиров Игорь Вакильевич</t>
+  </si>
+  <si>
+    <t>Баласанов Андрей Евгеньевич</t>
+  </si>
+  <si>
+    <t>Барабаш Кирилл Владимирович</t>
+  </si>
+  <si>
+    <t>Баронова Мария Николаевна</t>
+  </si>
+  <si>
+    <t>Беззуб Алексей Юрьевич</t>
+  </si>
+  <si>
+    <t>Безруких Олег Анатольевич</t>
+  </si>
+  <si>
+    <t>Билунов Денис Борисович</t>
+  </si>
+  <si>
+    <t>Блиндул Алексей Валерьевич</t>
+  </si>
+  <si>
+    <t>Брусиловский Максим Анатольевич</t>
+  </si>
+  <si>
+    <t>Будникова Софья Владимировна</t>
+  </si>
+  <si>
+    <t>Быстров Андрей Сергеевич</t>
+  </si>
+  <si>
+    <t>Васильева Елена Борисовна</t>
+  </si>
+  <si>
+    <t>Виноградов Сергей Николаевич</t>
+  </si>
+  <si>
+    <t>Винокуров Александр Иванович</t>
+  </si>
+  <si>
+    <t>Витухновская Алина Александровна</t>
+  </si>
+  <si>
+    <t>Власов Сергей Игоревич</t>
+  </si>
+  <si>
+    <t>Гаврилов Андрей Игоревич</t>
+  </si>
+  <si>
+    <t>Газарян Сурен Владимирович</t>
+  </si>
+  <si>
+    <t>Галямина Юлия Евгеньевна</t>
+  </si>
+  <si>
+    <t>Гарначук Владимир Федорович</t>
+  </si>
+  <si>
+    <t>Гельфанд Михаил Сергеевич</t>
+  </si>
+  <si>
+    <t>Глускин Владимир Александрович</t>
+  </si>
+  <si>
+    <t>Головин Дмитрий Александрович</t>
+  </si>
+  <si>
+    <t>Гонгальский Максим Брониславович</t>
+  </si>
+  <si>
+    <t>Горник Александр Львович</t>
+  </si>
+  <si>
+    <t>Готсданкер Алексей Сергеевич</t>
+  </si>
+  <si>
+    <t>Гребнева Ирина Георгиевна</t>
+  </si>
+  <si>
+    <t>Давыденко Денис Вячеславович</t>
+  </si>
+  <si>
+    <t>Давыдов Андрей Владимирович</t>
+  </si>
+  <si>
+    <t>Дегтярь Иван Васильевич</t>
+  </si>
+  <si>
+    <t>Демидов Михаил Александрович</t>
+  </si>
+  <si>
+    <t>Дергачев Вадим Александрович</t>
+  </si>
+  <si>
+    <t>Дзядко Филипп Викторович</t>
+  </si>
+  <si>
+    <t>Доможиров Евгений Валерьевич</t>
+  </si>
+  <si>
+    <t>Езеев Федор Андреевич</t>
+  </si>
+  <si>
+    <t>Зорин Константин Игоревич</t>
+  </si>
+  <si>
+    <t>Иванов Андрей Геннадьевич</t>
+  </si>
+  <si>
+    <t>Илларионов Андрей Николаевич</t>
+  </si>
+  <si>
+    <t>Кара-Мурза Владимир Владимирович</t>
+  </si>
+  <si>
+    <t>Каржаева Неонила Васильевна</t>
+  </si>
+  <si>
+    <t>Каспаров Гарри Кимович</t>
+  </si>
+  <si>
+    <t>Кац Максим Евгеньевич</t>
+  </si>
+  <si>
+    <t>Кашин Олег Владимирович</t>
+  </si>
+  <si>
+    <t>Козырев Олег Вилисович</t>
+  </si>
+  <si>
+    <t>Колчинцев Вадим Валерьевич</t>
+  </si>
+  <si>
+    <t>Крашенинников Федор Геннадиевич</t>
+  </si>
+  <si>
+    <t>Крылов Олег Анатольевич</t>
+  </si>
+  <si>
+    <t>Крюков Василий Анатольевич</t>
+  </si>
+  <si>
+    <t>Кузин Евгений Андреевич</t>
+  </si>
+  <si>
+    <t>Кузнецов Андрей Владимирович</t>
+  </si>
+  <si>
+    <t>Курамшин Владимир Вячеславович</t>
+  </si>
+  <si>
+    <t>Лавров Андрей Валерьевич</t>
+  </si>
+  <si>
+    <t>Лазуренко (Северский) Артем Сергеевич</t>
+  </si>
+  <si>
+    <t>Левченко Екатерина Валентиновна</t>
+  </si>
+  <si>
+    <t>Левшиц Николай Дмитриевич</t>
+  </si>
+  <si>
+    <t>Литвинов Георгий Александрович (Артём Драгунов)</t>
+  </si>
+  <si>
+    <t>Магкоева Белла (Изабель) Казбековна</t>
+  </si>
+  <si>
+    <t>Малышев Владимир Эдуардович</t>
+  </si>
+  <si>
+    <t>Мальцева Анастасия Анатольевна (Анастасия Хрустальная)</t>
+  </si>
+  <si>
+    <t>Матвеев Михаил Николаевич</t>
+  </si>
+  <si>
+    <t>Мирзоев Владимир Владимирович</t>
+  </si>
+  <si>
+    <t>Митюшкина Надежда Львовна</t>
+  </si>
+  <si>
+    <t>Мокшанов Александр Александрович</t>
+  </si>
+  <si>
+    <t>Мухин Юрий Игнатьевич</t>
+  </si>
+  <si>
+    <t>Некрасов Дмитрий Александрович</t>
+  </si>
+  <si>
+    <t>Образцова Алиса Сергеевна</t>
+  </si>
+  <si>
+    <t>Овдиенко Игорь Геннадьевич</t>
+  </si>
+  <si>
+    <t>Ольшанский Леонид Дмитриевич</t>
+  </si>
+  <si>
+    <t>Осенин Владимир Олегович</t>
+  </si>
+  <si>
+    <t>Отставных Валерий Владимирович</t>
+  </si>
+  <si>
+    <t>Пархоменко Сергей Борисович</t>
+  </si>
+  <si>
+    <t>Первушин Александр Сергеевич</t>
+  </si>
+  <si>
+    <t>Петречук Лариса Леонидовна</t>
+  </si>
+  <si>
+    <t>Пионтковский Андрей Андреевич</t>
+  </si>
+  <si>
+    <t>Поляков Анатолий Викторович</t>
+  </si>
+  <si>
+    <t>Пономарев Илья Владимирович</t>
+  </si>
+  <si>
+    <t>Поткин (Басманов) Владимир Анатольевич</t>
+  </si>
+  <si>
+    <t>Пряников Павел Николаевич</t>
+  </si>
+  <si>
+    <t>Ренёв Денис Владимирович</t>
+  </si>
+  <si>
+    <t>Русакова Елена Леонидовна</t>
+  </si>
+  <si>
+    <t>Савостин Михаил Олегович</t>
+  </si>
+  <si>
+    <t>Сайдашев Радик Ромович</t>
+  </si>
+  <si>
+    <t>Семенов Владимир Матвеевич</t>
+  </si>
+  <si>
+    <t>Семенов Игорь Вячеславович</t>
+  </si>
+  <si>
+    <t>Скалаух Иван Сергеевич</t>
+  </si>
+  <si>
+    <t>Смирнов Сергей Сергеевич</t>
+  </si>
+  <si>
+    <t>Спорыхина Ульяна Викторовна</t>
+  </si>
+  <si>
+    <t>Стефанов Борис Александрович</t>
+  </si>
+  <si>
+    <t>Сухарева Татьяна Викторовна</t>
+  </si>
+  <si>
+    <t>Терегулов Артур Ринатович</t>
+  </si>
+  <si>
+    <t>Удальцова Анастасия Олеговна</t>
+  </si>
+  <si>
+    <t>Чупров Алексей Геннадьевич</t>
+  </si>
+  <si>
+    <t>Шатов Станислав Николаевич</t>
+  </si>
+  <si>
+    <t>Шац Михаил Григорьевич</t>
+  </si>
+  <si>
+    <t>Шнейдер Михаил Яковлевич</t>
+  </si>
+  <si>
+    <t>Щербаков Александр Вениаминович</t>
+  </si>
+  <si>
+    <t>Эсауленко Дмитрий Николаевич</t>
+  </si>
+  <si>
+    <t>Янкаускас Константин Стасисович</t>
+  </si>
+  <si>
+    <t>Яшин (Ясин) Игорь Геннадьевич</t>
+  </si>
+  <si>
+    <t>Аитова Екатерина Петровна</t>
+  </si>
+  <si>
+    <t>Волкова Александра Ивановна (Женя Отто)</t>
+  </si>
+  <si>
+    <t>Николаев Александр Александрович</t>
+  </si>
+  <si>
+    <t>Печенев Александр Сергеевич</t>
+  </si>
+  <si>
+    <t>Санников Максим Андреевич</t>
+  </si>
+  <si>
+    <t>Шалимов Роман Николаевич</t>
+  </si>
+  <si>
+    <t>Давидис Сергей Константинович</t>
+  </si>
+  <si>
+    <t>Долгих Антон Витальевич</t>
+  </si>
+  <si>
+    <t>Залесский Александр Валерьевич</t>
+  </si>
+  <si>
+    <t>Пивоваров Андрей Сергеевич</t>
+  </si>
+  <si>
+    <t>Тютрин Иван Иванович</t>
+  </si>
+  <si>
+    <t>Шальнев Андрей Сергеевич</t>
+  </si>
+  <si>
+    <t>Артёмов Игорь Владимирович</t>
+  </si>
+  <si>
+    <t>Демушкин Дмитрий Николаевич</t>
+  </si>
+  <si>
+    <t>Дровецкий Василий Валерьевич</t>
+  </si>
+  <si>
+    <t>Крылов Константин Анатольевич</t>
   </si>
 </sst>
 </file>
@@ -795,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA172"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131:XFD132"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162:G175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,6 +1255,9 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
@@ -975,6 +1335,9 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1052,6 +1415,9 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -1129,6 +1495,9 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1206,6 +1575,9 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1283,6 +1655,9 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -1360,6 +1735,9 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
@@ -1437,6 +1815,9 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -1514,6 +1895,9 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
@@ -1591,6 +1975,9 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1668,6 +2055,9 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -1745,6 +2135,9 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -1822,6 +2215,9 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" s="1">
         <v>-2</v>
       </c>
@@ -1899,6 +2295,9 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -1976,6 +2375,9 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -2052,7 +2454,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
@@ -2129,7 +2534,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B18" s="1">
         <v>-2</v>
       </c>
@@ -2206,7 +2614,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -2283,7 +2694,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
@@ -2360,7 +2774,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B21" s="1">
         <v>-1</v>
       </c>
@@ -2437,7 +2854,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B22" s="1">
         <v>-2</v>
       </c>
@@ -2514,7 +2934,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -2591,7 +3014,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -2668,7 +3094,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
@@ -2745,7 +3174,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
@@ -2822,7 +3254,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B27" s="1">
         <v>-1</v>
       </c>
@@ -2899,7 +3334,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
@@ -2976,7 +3414,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
@@ -3053,7 +3494,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B30" s="1">
         <v>-1</v>
       </c>
@@ -3130,7 +3574,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B31" s="1">
         <v>2</v>
       </c>
@@ -3207,7 +3654,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
@@ -3284,7 +3734,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B33" s="1">
         <v>-1</v>
       </c>
@@ -3361,7 +3814,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B34" s="1">
         <v>2</v>
       </c>
@@ -3438,7 +3894,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
@@ -3515,7 +3974,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B36" s="1">
         <v>-2</v>
       </c>
@@ -3592,7 +4054,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B37" s="1">
         <v>2</v>
       </c>
@@ -3669,7 +4134,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
@@ -3746,7 +4214,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
@@ -3823,7 +4294,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="B40" s="1">
         <v>2</v>
       </c>
@@ -3900,7 +4374,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B41" s="1">
         <v>-1</v>
       </c>
@@ -3977,7 +4454,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B42" s="1">
         <v>-1</v>
       </c>
@@ -4054,7 +4534,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B43" s="1">
         <v>2</v>
       </c>
@@ -4131,7 +4614,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B44" s="1">
         <v>2</v>
       </c>
@@ -4208,7 +4694,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B45" s="1">
         <v>2</v>
       </c>
@@ -4285,7 +4774,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B46" s="1">
         <v>1</v>
       </c>
@@ -4362,7 +4854,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B47" s="1">
         <v>2</v>
       </c>
@@ -4439,7 +4934,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B48" s="1">
         <v>1</v>
       </c>
@@ -4516,7 +5014,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="B49" s="1">
         <v>1</v>
       </c>
@@ -4593,7 +5094,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="B50" s="1">
         <v>-2</v>
       </c>
@@ -4670,7 +5174,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B51" s="1">
         <v>2</v>
       </c>
@@ -4747,7 +5254,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B52" s="1">
         <v>-1</v>
       </c>
@@ -4824,7 +5334,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B53" s="1">
         <v>1</v>
       </c>
@@ -4901,7 +5414,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="B54" s="1">
         <v>2</v>
       </c>
@@ -4978,7 +5494,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B55" s="1">
         <v>-1</v>
       </c>
@@ -5055,7 +5574,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B56" s="1">
         <v>-1</v>
       </c>
@@ -5132,7 +5654,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B57" s="1">
         <v>2</v>
       </c>
@@ -5209,7 +5734,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B58" s="1">
         <v>2</v>
       </c>
@@ -5286,7 +5814,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B59" s="1">
         <v>2</v>
       </c>
@@ -5363,7 +5894,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B60" s="1">
         <v>1</v>
       </c>
@@ -5440,7 +5974,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B61" s="1">
         <v>1</v>
       </c>
@@ -5517,7 +6054,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B62" s="1">
         <v>-2</v>
       </c>
@@ -5594,7 +6134,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="63" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
@@ -5671,7 +6214,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B64" s="1">
         <v>-2</v>
       </c>
@@ -5748,7 +6294,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B65" s="1">
         <v>-1</v>
       </c>
@@ -5825,7 +6374,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="B66" s="1">
         <v>2</v>
       </c>
@@ -5902,7 +6454,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B67" s="1">
         <v>1</v>
       </c>
@@ -5979,7 +6534,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="B68" s="1">
         <v>1</v>
       </c>
@@ -6056,7 +6614,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B69" s="1">
         <v>2</v>
       </c>
@@ -6133,7 +6694,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="70" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="B70" s="1">
         <v>1</v>
       </c>
@@ -6210,7 +6774,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="B71" s="1">
         <v>2</v>
       </c>
@@ -6287,7 +6854,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="72" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="B72" s="1">
         <v>2</v>
       </c>
@@ -6364,7 +6934,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B73" s="1">
         <v>2</v>
       </c>
@@ -6441,7 +7014,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="B74" s="1">
         <v>2</v>
       </c>
@@ -6518,7 +7094,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="B75" s="1">
         <v>0</v>
       </c>
@@ -6595,7 +7174,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="B76" s="1">
         <v>-1</v>
       </c>
@@ -6672,7 +7254,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="B77" s="1">
         <v>2</v>
       </c>
@@ -6749,7 +7334,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="78" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="B78" s="1">
         <v>2</v>
       </c>
@@ -6826,7 +7414,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="B79" s="1">
         <v>2</v>
       </c>
@@ -6903,7 +7494,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="B80" s="1">
         <v>2</v>
       </c>
@@ -6980,7 +7574,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="81" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="B81" s="1">
         <v>2</v>
       </c>
@@ -7057,7 +7654,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B82" s="1">
         <v>0</v>
       </c>
@@ -7134,7 +7734,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="83" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B83" s="1">
         <v>2</v>
       </c>
@@ -7211,7 +7814,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B84" s="1">
         <v>-1</v>
       </c>
@@ -7288,7 +7894,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="B85" s="1">
         <v>2</v>
       </c>
@@ -7365,7 +7974,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="B86" s="1">
         <v>2</v>
       </c>
@@ -7442,7 +8054,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="B87" s="1">
         <v>2</v>
       </c>
@@ -7519,7 +8134,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="B88" s="1">
         <v>2</v>
       </c>
@@ -7596,7 +8214,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B89" s="1">
         <v>1</v>
       </c>
@@ -7673,7 +8294,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="B90" s="1">
         <v>2</v>
       </c>
@@ -7750,7 +8374,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B91" s="1">
         <v>2</v>
       </c>
@@ -7827,7 +8454,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="92" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="B92" s="1">
         <v>1</v>
       </c>
@@ -7904,7 +8534,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B93" s="1">
         <v>1</v>
       </c>
@@ -7981,7 +8614,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="B94" s="1">
         <v>1</v>
       </c>
@@ -8058,7 +8694,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="95" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="B95" s="1">
         <v>0</v>
       </c>
@@ -8135,7 +8774,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="B96" s="1">
         <v>2</v>
       </c>
@@ -8212,7 +8854,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="B97" s="1">
         <v>2</v>
       </c>
@@ -8289,7 +8934,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="98" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="B98" s="1">
         <v>-1</v>
       </c>
@@ -8366,7 +9014,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="B99" s="1">
         <v>-1</v>
       </c>
@@ -8443,7 +9094,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="100" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B100" s="1">
         <v>1</v>
       </c>
@@ -8520,7 +9174,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B101" s="1">
         <v>2</v>
       </c>
@@ -8597,7 +9254,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="B102" s="1">
         <v>2</v>
       </c>
@@ -8674,7 +9334,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="B103" s="1">
         <v>1</v>
       </c>
@@ -8751,7 +9414,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="B104" s="1">
         <v>1</v>
       </c>
@@ -8828,7 +9494,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="105" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B105" s="1">
         <v>1</v>
       </c>
@@ -8905,7 +9574,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B106" s="1">
         <v>1</v>
       </c>
@@ -8982,7 +9654,10 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="107" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B107" s="1">
         <v>-1</v>
       </c>
@@ -9059,7 +9734,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="B108" s="1">
         <v>1</v>
       </c>
@@ -9136,7 +9814,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="B109" s="1">
         <v>1</v>
       </c>
@@ -9213,7 +9894,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B110" s="1">
         <v>-1</v>
       </c>
@@ -9290,7 +9974,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="B111" s="1">
         <v>1</v>
       </c>
@@ -9367,7 +10054,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="112" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="B112" s="1">
         <v>2</v>
       </c>
@@ -9445,6 +10135,9 @@
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="B113" s="1">
         <v>1</v>
       </c>
@@ -9522,6 +10215,9 @@
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="B114" s="1">
         <v>1</v>
       </c>
@@ -9599,6 +10295,9 @@
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="B115" s="1">
         <v>2</v>
       </c>
@@ -9676,6 +10375,9 @@
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="B116" s="1">
         <v>2</v>
       </c>
@@ -9753,6 +10455,9 @@
       </c>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B117" s="1">
         <v>1</v>
       </c>
@@ -9830,6 +10535,9 @@
       </c>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="B118" s="1">
         <v>-1</v>
       </c>
@@ -9907,6 +10615,9 @@
       </c>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="B119" s="1">
         <v>2</v>
       </c>
@@ -9984,6 +10695,9 @@
       </c>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="B120" s="1">
         <v>0</v>
       </c>
@@ -13462,57 +14176,33 @@
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4">
-        <v>2</v>
-      </c>
-      <c r="C163" s="4">
-        <v>2</v>
-      </c>
-      <c r="D163" s="4">
-        <v>2</v>
-      </c>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4">
-        <v>6</v>
-      </c>
-      <c r="C164" s="4">
-        <v>18</v>
-      </c>
-      <c r="D164" s="4">
-        <v>-11</v>
-      </c>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4">
-        <v>7</v>
-      </c>
-      <c r="C165" s="4">
-        <v>19</v>
-      </c>
-      <c r="D165" s="4">
-        <v>-24</v>
-      </c>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="4"/>
-      <c r="C166" s="4">
-        <v>-24</v>
-      </c>
+      <c r="C166" s="4"/>
       <c r="D166" s="4"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="4"/>
-      <c r="C167" s="4">
-        <v>-11</v>
-      </c>
+      <c r="C167" s="4"/>
       <c r="D167" s="4"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="4"/>
-      <c r="C168" s="4">
-        <v>-10</v>
-      </c>
+      <c r="C168" s="4"/>
       <c r="D168" s="4"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
@@ -13622,8 +14312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>